<commit_message>
added little more delay in files
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Phone</t>
   </si>
@@ -28,13 +28,10 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Company</t>
-  </si>
-  <si>
     <t xml:space="preserve">State</t>
   </si>
   <si>
-    <t xml:space="preserve">Enquiry For</t>
+    <t xml:space="preserve">Template Name</t>
   </si>
   <si>
     <t xml:space="preserve">Enquiry From</t>
@@ -43,22 +40,25 @@
     <t xml:space="preserve">Sonu Pal</t>
   </si>
   <si>
-    <t xml:space="preserve">Lv Enterprises</t>
+    <t xml:space="preserve">Rajasthan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAVANYA_HINDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indiamart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shilpi</t>
   </si>
   <si>
     <t xml:space="preserve">Delhi</t>
   </si>
   <si>
-    <t xml:space="preserve">Soft Toys</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trade India</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shilpi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LV T</t>
+    <t xml:space="preserve">LAVANYA_ENGLISH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exporters India</t>
   </si>
 </sst>
 </file>
@@ -160,15 +160,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.31640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="17.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -187,28 +187,22 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>7503085792</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -216,19 +210,16 @@
         <v>9870117763</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>